<commit_message>
Incorporate additional fixes from WRI
</commit_message>
<xml_diff>
--- a/InputData/elec/MPCbS/Max Potential Capacity by Source.xlsx
+++ b/InputData/elec/MPCbS/Max Potential Capacity by Source.xlsx
@@ -9,20 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11220"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Biomass" sheetId="6" r:id="rId2"/>
     <sheet name="MSW" sheetId="7" r:id="rId3"/>
-    <sheet name="MPCbS" sheetId="3" r:id="rId4"/>
+    <sheet name="Pumped Hydro" sheetId="8" r:id="rId4"/>
+    <sheet name="MPCbS" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="111">
   <si>
     <t>MPCbS Max Potential Capacity by Source</t>
   </si>
@@ -349,6 +352,24 @@
   </si>
   <si>
     <t>Source: Gujarat ENVIS Centre</t>
+  </si>
+  <si>
+    <t>Pumped Hydro</t>
+  </si>
+  <si>
+    <t>Central Electricity Authority/Ministry of Power</t>
+  </si>
+  <si>
+    <t>Minutes of the meeting regarding operationalization of existing pump storage plants held on 28th June, 2017</t>
+  </si>
+  <si>
+    <t>http://www.cea.nic.in/reports/others/planning/resd/mom_pump_storage_plants.pdf</t>
+  </si>
+  <si>
+    <t>Page 4</t>
+  </si>
+  <si>
+    <t>Potential</t>
   </si>
 </sst>
 </file>
@@ -485,6 +506,55 @@
         <a:xfrm>
           <a:off x="5849972" y="0"/>
           <a:ext cx="5809403" cy="5829299"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>419924</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>143134</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6BF28FB-9B84-4CD6-BA4C-D2EE024A3CCF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4267200" y="0"/>
+          <a:ext cx="5906324" cy="1857634"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -785,7 +855,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -853,98 +925,134 @@
       <c r="B10" s="2" t="s">
         <v>74</v>
       </c>
+      <c r="F10" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>2</v>
       </c>
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B12" s="3">
         <v>2017</v>
       </c>
+      <c r="F12" s="3">
+        <v>2017</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>3</v>
       </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="F14" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="F15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B17" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="F17" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B18" s="7" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="F18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B19" s="3">
         <v>2016</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="F19" s="3">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="F20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="F21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="F22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>85</v>
       </c>
@@ -958,9 +1066,10 @@
   <hyperlinks>
     <hyperlink ref="B14" r:id="rId1"/>
     <hyperlink ref="B7" r:id="rId2"/>
+    <hyperlink ref="F14" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -968,7 +1077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
@@ -1990,13 +2099,52 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>96524</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2088,8 +2236,8 @@
         <v>11</v>
       </c>
       <c r="B10" s="5">
-        <f>B5</f>
-        <v>163000</v>
+        <f>'Pumped Hydro'!A2</f>
+        <v>96524</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Update max capacity variables
</commit_message>
<xml_diff>
--- a/InputData/elec/MPCbS/Max Potential Capacity by Source.xlsx
+++ b/InputData/elec/MPCbS/Max Potential Capacity by Source.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\elec\MPCbS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-india\InputData\elec\MPCbS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,10 +15,12 @@
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Biomass" sheetId="6" r:id="rId2"/>
     <sheet name="MSW" sheetId="7" r:id="rId3"/>
-    <sheet name="Pumped Hydro" sheetId="8" r:id="rId4"/>
-    <sheet name="MPCbS" sheetId="3" r:id="rId5"/>
+    <sheet name="Onshore Wind" sheetId="10" r:id="rId4"/>
+    <sheet name="Solar PV" sheetId="9" r:id="rId5"/>
+    <sheet name="Pumped Hydro" sheetId="8" r:id="rId6"/>
+    <sheet name="MPCbS" sheetId="3" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="109">
   <si>
     <t>MPCbS Max Potential Capacity by Source</t>
   </si>
@@ -258,45 +260,18 @@
     <t>Appendix A2</t>
   </si>
   <si>
-    <t>All Except Biomass, Onshore Wind</t>
-  </si>
-  <si>
     <t>Biomass</t>
   </si>
   <si>
-    <t>file:///C:/Users/deept/AppData/Local/Temp/CSTEP_RR_Re-assessment_of_India's_On-shore_Wind_Power_Potential_2016.pdf</t>
-  </si>
-  <si>
-    <t>Onshore Wind</t>
-  </si>
-  <si>
     <t>Source: MNRE</t>
   </si>
   <si>
     <t>Source: CSTEP, WFMS, SSEF</t>
   </si>
   <si>
-    <t>(5Dx7D array potential - conservative)</t>
-  </si>
-  <si>
-    <t>Re-assessment of India’s On-shore Wind Power Potential</t>
-  </si>
-  <si>
-    <t>CSTEP, WFMS, SSEF - for MNRE's Wind Potential Reassessment Committee</t>
-  </si>
-  <si>
-    <t>Appendix 2, pp 61</t>
-  </si>
-  <si>
     <t>Notes:</t>
   </si>
   <si>
-    <t>On-shore wind potential has been reassessed by CSTEP, WFMS &amp; SSEF study as part of MNRE's Potential Re-assessment committee in 2016</t>
-  </si>
-  <si>
-    <t>New estimate of on-shore wind potential for 100m hub height is considered, for a conservative wind farm array configuration of 5Dx7D</t>
-  </si>
-  <si>
     <t>be geographically resource-constrained. (An arbitrarily high number is chosen here, to ensure</t>
   </si>
   <si>
@@ -345,9 +320,6 @@
     <t>municipal solid waste</t>
   </si>
   <si>
-    <t>Remaining sources from TERI-WWF study, except for Biomass and MSW from MNRE latest available potential estimate.</t>
-  </si>
-  <si>
     <t>Page 4, in lieu of MNRE source no longer available on their site</t>
   </si>
   <si>
@@ -370,12 +342,39 @@
   </si>
   <si>
     <t>Potential</t>
+  </si>
+  <si>
+    <t>All Except Biomass, Onshore Wind, Solar PV, Pumped Hydro</t>
+  </si>
+  <si>
+    <t>Onshore Wind and Solar</t>
+  </si>
+  <si>
+    <t>U.S. National Renewable Energy Laboratory</t>
+  </si>
+  <si>
+    <t>Renewable Energy Data Explorer</t>
+  </si>
+  <si>
+    <t>For wind and solar, we ran NREL's Renewable Energy Data Explorer tool, using the suggested</t>
+  </si>
+  <si>
+    <t>default parameters.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.re-explorer.org/ </t>
+  </si>
+  <si>
+    <t>Analysis and Downloads tab accessed 1/29/2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -436,7 +435,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -450,6 +449,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -518,6 +518,168 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>104776</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>65719</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>626323</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>109538</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="104776" y="65719"/>
+          <a:ext cx="9589347" cy="4930144"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>149311</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>30974</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>109538</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9864811" y="66675"/>
+          <a:ext cx="9597163" cy="4929188"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>465540</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>18444</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="57150" y="57150"/>
+          <a:ext cx="9476190" cy="4847619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>642937</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>388162</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>3779</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9710737" y="47625"/>
+          <a:ext cx="9460725" cy="4842479"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -853,10 +1015,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -875,10 +1037,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -886,7 +1048,7 @@
         <v>69</v>
       </c>
       <c r="F4" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -894,7 +1056,7 @@
         <v>2011</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -902,7 +1064,7 @@
         <v>70</v>
       </c>
       <c r="F6" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -910,7 +1072,7 @@
         <v>71</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -918,15 +1080,15 @@
         <v>72</v>
       </c>
       <c r="F8" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -971,23 +1133,23 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B17" s="2" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B18" s="7" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="F18" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B19" s="3">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="F19" s="3">
         <v>2017</v>
@@ -995,71 +1157,61 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="F20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B21" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B21" t="s">
-        <v>75</v>
-      </c>
       <c r="F21" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="F22" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B23" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1067,9 +1219,10 @@
     <hyperlink ref="B14" r:id="rId1"/>
     <hyperlink ref="B7" r:id="rId2"/>
     <hyperlink ref="F14" r:id="rId3"/>
+    <hyperlink ref="B21" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1792,7 +1945,7 @@
         <v>2131</v>
       </c>
       <c r="K29" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.45">
@@ -2040,7 +2193,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2061,34 +2214,34 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B2">
         <v>1700</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B3">
         <v>1300</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2098,6 +2251,56 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A29:B29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29">
+        <f>9*1000000</f>
+        <v>9000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A29:B29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29">
+        <f>98*1000000</f>
+        <v>98000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
@@ -2109,7 +2312,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
@@ -2117,17 +2320,17 @@
         <v>96524</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="H11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="H12" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2136,15 +2339,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2153,7 +2356,7 @@
     <col min="2" max="2" width="27.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
@@ -2161,7 +2364,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -2170,7 +2373,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -2179,7 +2382,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -2188,7 +2391,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2197,32 +2400,34 @@
         <v>163000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>2760000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <f>'Onshore Wind'!$B$29</f>
+        <v>9000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>1400000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+        <f>'Solar PV'!B29</f>
+        <v>98000000</v>
+      </c>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="5">
-        <f>B7</f>
         <v>1400000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2231,7 +2436,7 @@
         <v>25090</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -2240,7 +2445,7 @@
         <v>96524</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>66</v>
       </c>
@@ -2249,7 +2454,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -2258,7 +2463,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -2267,7 +2472,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
@@ -2275,18 +2480,18 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B15" s="6">
         <f>B11</f>
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B16" s="6">
         <f>B11</f>
@@ -2295,7 +2500,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B17" s="6">
         <f>MSW!B2+MSW!B3</f>

</xml_diff>